<commit_message>
feat: arquivos e resultados dos modelos adicionados
</commit_message>
<xml_diff>
--- a/Dataset.xlsx
+++ b/Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\OneDrive\Área de Trabalho\folhasAmendoim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FE0805-1E2F-4AF7-BBD7-82AAFAD4E8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE6E1E5-ED8F-4528-A4D8-A2899A3CF9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1430,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="B344" sqref="B344"/>
+    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
+      <selection activeCell="P350" sqref="P350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>